<commit_message>
fix the farm id
</commit_message>
<xml_diff>
--- a/data/TASK 2.3.4 2023-2024 - Flusso Azienda.xlsx
+++ b/data/TASK 2.3.4 2023-2024 - Flusso Azienda.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveunibo-my.sharepoint.com/personal/matteo_francia2_studio_unibo_it/Documents/Documents/repos/dataset-pnrr-spoke2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{862CA7C1-3C51-433E-909D-DF07B5BDFC70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F1F2EC80-33B8-4494-A106-4354147EC8B6}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{862CA7C1-3C51-433E-909D-DF07B5BDFC70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF7F27C6-26EE-4941-9C29-C963440EA9BE}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1250" windowWidth="9850" windowHeight="4300" xr2:uid="{06003F17-5CB1-44B8-838E-5C3C1E26A2CC}"/>
+    <workbookView xWindow="13050" yWindow="4320" windowWidth="9840" windowHeight="12380" xr2:uid="{06003F17-5CB1-44B8-838E-5C3C1E26A2CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -473,17 +473,17 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.81640625" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -497,7 +497,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>7</v>
       </c>
@@ -511,7 +511,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>8</v>
       </c>
@@ -525,7 +525,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>9</v>
       </c>
@@ -539,7 +539,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -553,9 +553,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>3</v>
@@ -567,7 +567,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -588,15 +588,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101003AD0A2D44F687740A29D74EB23F0CEDB" ma:contentTypeVersion="16" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="0cbee3a7b31ef12ad080c50c46137e00">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8d0ad65a-05b0-4576-ba97-3fba7ef64242" xmlns:ns3="ec9f8fc5-8766-4d78-a9a6-acc81b8e5366" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="95ce5791b71b5371617f4d3b4579cad3" ns2:_="" ns3:_="">
     <xsd:import namespace="8d0ad65a-05b0-4576-ba97-3fba7ef64242"/>
@@ -837,6 +828,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -849,14 +849,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{477CC755-13A3-436B-B88A-B0134F92DB87}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7EC2EBA5-2A74-46BC-9C1F-08B0D0BBDDD8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -875,6 +867,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{477CC755-13A3-436B-B88A-B0134F92DB87}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CEB70741-19FE-4435-8099-1C3681608AF5}">
   <ds:schemaRefs>

</xml_diff>